<commit_message>
fixed some more takes data
</commit_message>
<xml_diff>
--- a/data/Excel Format/relations/Takes.xlsx
+++ b/data/Excel Format/relations/Takes.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2157" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2151" uniqueCount="93">
   <si>
     <t>ID</t>
   </si>
@@ -271,7 +271,7 @@
     <t>ERS 106</t>
   </si>
   <si>
-    <t>GER 271</t>
+    <t>MSCI 211</t>
   </si>
   <si>
     <t>ECE 204</t>
@@ -365,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -400,6 +400,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -10173,17 +10176,17 @@
       <c r="B480" s="5">
         <v>1.2345677E7</v>
       </c>
-      <c r="C480" s="6" t="s">
-        <v>56</v>
+      <c r="C480" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="D480" s="5">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E480" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F480" s="5">
-        <v>2023.0</v>
+        <v>2021.0</v>
       </c>
       <c r="G480" s="1" t="s">
         <v>8</v>
@@ -10194,7 +10197,7 @@
         <v>1.2345677E7</v>
       </c>
       <c r="C481" s="4" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="D481" s="5">
         <v>1.0</v>
@@ -10203,7 +10206,7 @@
         <v>14</v>
       </c>
       <c r="F481" s="5">
-        <v>2020.0</v>
+        <v>2021.0</v>
       </c>
       <c r="G481" s="1" t="s">
         <v>8</v>
@@ -10213,8 +10216,8 @@
       <c r="B482" s="5">
         <v>1.2345677E7</v>
       </c>
-      <c r="C482" s="9" t="s">
-        <v>15</v>
+      <c r="C482" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="D482" s="5">
         <v>1.0</v>
@@ -10222,8 +10225,8 @@
       <c r="E482" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F482" s="7">
-        <v>2021.0</v>
+      <c r="F482" s="13">
+        <v>2022.0</v>
       </c>
       <c r="G482" s="1" t="s">
         <v>16</v>
@@ -10234,7 +10237,7 @@
         <v>1.2345677E7</v>
       </c>
       <c r="C483" s="4" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="D483" s="5">
         <v>1.0</v>
@@ -10243,7 +10246,7 @@
         <v>7</v>
       </c>
       <c r="F483" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G483" s="2" t="s">
         <v>19</v>
@@ -10254,7 +10257,7 @@
         <v>1.2345677E7</v>
       </c>
       <c r="C484" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D484" s="5">
         <v>1.0</v>
@@ -10263,7 +10266,7 @@
         <v>7</v>
       </c>
       <c r="F484" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G484" s="2" t="s">
         <v>19</v>
@@ -10274,7 +10277,7 @@
         <v>1.2345677E7</v>
       </c>
       <c r="C485" s="4" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="D485" s="5">
         <v>1.0</v>
@@ -10283,7 +10286,7 @@
         <v>14</v>
       </c>
       <c r="F485" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G485" s="2" t="s">
         <v>27</v>
@@ -10294,7 +10297,7 @@
         <v>1.2345677E7</v>
       </c>
       <c r="C486" s="4" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="D486" s="5">
         <v>1.0</v>
@@ -10303,7 +10306,7 @@
         <v>7</v>
       </c>
       <c r="F486" s="5">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="G486" s="2" t="s">
         <v>32</v>
@@ -10313,8 +10316,8 @@
       <c r="B487" s="5">
         <v>1.2345677E7</v>
       </c>
-      <c r="C487" s="4" t="s">
-        <v>10</v>
+      <c r="C487" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="D487" s="5">
         <v>1.0</v>
@@ -10323,7 +10326,7 @@
         <v>7</v>
       </c>
       <c r="F487" s="5">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="G487" s="2" t="s">
         <v>32</v>
@@ -10337,7 +10340,7 @@
         <v>11</v>
       </c>
       <c r="D488" s="5">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="E488" s="4" t="s">
         <v>14</v>
@@ -10353,17 +10356,17 @@
       <c r="B489" s="5">
         <v>2.1487654E7</v>
       </c>
-      <c r="C489" s="6" t="s">
-        <v>56</v>
+      <c r="C489" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="D489" s="5">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E489" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F489" s="5">
-        <v>2023.0</v>
+        <v>2021.0</v>
       </c>
       <c r="G489" s="1" t="s">
         <v>8</v>
@@ -10374,7 +10377,7 @@
         <v>2.1487654E7</v>
       </c>
       <c r="C490" s="4" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="D490" s="5">
         <v>1.0</v>
@@ -10383,7 +10386,7 @@
         <v>14</v>
       </c>
       <c r="F490" s="5">
-        <v>2020.0</v>
+        <v>2021.0</v>
       </c>
       <c r="G490" s="1" t="s">
         <v>8</v>
@@ -10393,8 +10396,8 @@
       <c r="B491" s="5">
         <v>2.1487654E7</v>
       </c>
-      <c r="C491" s="9" t="s">
-        <v>15</v>
+      <c r="C491" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="D491" s="5">
         <v>1.0</v>
@@ -10402,8 +10405,8 @@
       <c r="E491" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F491" s="7">
-        <v>2021.0</v>
+      <c r="F491" s="13">
+        <v>2022.0</v>
       </c>
       <c r="G491" s="1" t="s">
         <v>16</v>
@@ -10414,7 +10417,7 @@
         <v>2.1487654E7</v>
       </c>
       <c r="C492" s="4" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="D492" s="5">
         <v>1.0</v>
@@ -10423,7 +10426,7 @@
         <v>7</v>
       </c>
       <c r="F492" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G492" s="2" t="s">
         <v>19</v>
@@ -10434,7 +10437,7 @@
         <v>2.1487654E7</v>
       </c>
       <c r="C493" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D493" s="5">
         <v>1.0</v>
@@ -10443,7 +10446,7 @@
         <v>7</v>
       </c>
       <c r="F493" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G493" s="2" t="s">
         <v>19</v>
@@ -10454,7 +10457,7 @@
         <v>2.1487654E7</v>
       </c>
       <c r="C494" s="4" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="D494" s="5">
         <v>1.0</v>
@@ -10463,7 +10466,7 @@
         <v>14</v>
       </c>
       <c r="F494" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G494" s="2" t="s">
         <v>27</v>
@@ -10474,7 +10477,7 @@
         <v>2.1487654E7</v>
       </c>
       <c r="C495" s="4" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="D495" s="5">
         <v>1.0</v>
@@ -10483,7 +10486,7 @@
         <v>7</v>
       </c>
       <c r="F495" s="5">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="G495" s="2" t="s">
         <v>32</v>
@@ -10493,8 +10496,8 @@
       <c r="B496" s="5">
         <v>2.1487654E7</v>
       </c>
-      <c r="C496" s="4" t="s">
-        <v>10</v>
+      <c r="C496" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="D496" s="5">
         <v>1.0</v>
@@ -10503,7 +10506,7 @@
         <v>7</v>
       </c>
       <c r="F496" s="5">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="G496" s="2" t="s">
         <v>32</v>
@@ -10514,10 +10517,10 @@
         <v>2.0928175E7</v>
       </c>
       <c r="C497" s="4" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="D497" s="5">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E497" s="4" t="s">
         <v>14</v>
@@ -10533,17 +10536,17 @@
       <c r="B498" s="5">
         <v>2.0928175E7</v>
       </c>
-      <c r="C498" s="6" t="s">
-        <v>56</v>
+      <c r="C498" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="D498" s="5">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E498" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F498" s="5">
-        <v>2023.0</v>
+        <v>2021.0</v>
       </c>
       <c r="G498" s="1" t="s">
         <v>8</v>
@@ -10554,7 +10557,7 @@
         <v>2.0928175E7</v>
       </c>
       <c r="C499" s="4" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="D499" s="5">
         <v>1.0</v>
@@ -10563,7 +10566,7 @@
         <v>14</v>
       </c>
       <c r="F499" s="5">
-        <v>2020.0</v>
+        <v>2021.0</v>
       </c>
       <c r="G499" s="1" t="s">
         <v>8</v>
@@ -10573,8 +10576,8 @@
       <c r="B500" s="5">
         <v>2.0928175E7</v>
       </c>
-      <c r="C500" s="9" t="s">
-        <v>15</v>
+      <c r="C500" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="D500" s="5">
         <v>1.0</v>
@@ -10582,8 +10585,8 @@
       <c r="E500" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F500" s="7">
-        <v>2021.0</v>
+      <c r="F500" s="13">
+        <v>2022.0</v>
       </c>
       <c r="G500" s="1" t="s">
         <v>16</v>
@@ -10594,7 +10597,7 @@
         <v>2.0928175E7</v>
       </c>
       <c r="C501" s="4" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="D501" s="5">
         <v>1.0</v>
@@ -10603,7 +10606,7 @@
         <v>7</v>
       </c>
       <c r="F501" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G501" s="2" t="s">
         <v>19</v>
@@ -10614,7 +10617,7 @@
         <v>2.0928175E7</v>
       </c>
       <c r="C502" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D502" s="5">
         <v>1.0</v>
@@ -10623,7 +10626,7 @@
         <v>7</v>
       </c>
       <c r="F502" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G502" s="2" t="s">
         <v>19</v>
@@ -10634,7 +10637,7 @@
         <v>2.0928175E7</v>
       </c>
       <c r="C503" s="4" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="D503" s="5">
         <v>1.0</v>
@@ -10643,7 +10646,7 @@
         <v>14</v>
       </c>
       <c r="F503" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G503" s="2" t="s">
         <v>27</v>
@@ -10654,7 +10657,7 @@
         <v>2.1765423E7</v>
       </c>
       <c r="C504" s="4" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="D504" s="5">
         <v>2.0</v>
@@ -10673,17 +10676,17 @@
       <c r="B505" s="5">
         <v>2.1765423E7</v>
       </c>
-      <c r="C505" s="6" t="s">
-        <v>56</v>
+      <c r="C505" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="D505" s="5">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E505" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F505" s="5">
-        <v>2023.0</v>
+        <v>2021.0</v>
       </c>
       <c r="G505" s="1" t="s">
         <v>8</v>
@@ -10694,7 +10697,7 @@
         <v>2.1765423E7</v>
       </c>
       <c r="C506" s="4" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="D506" s="5">
         <v>1.0</v>
@@ -10703,7 +10706,7 @@
         <v>14</v>
       </c>
       <c r="F506" s="5">
-        <v>2020.0</v>
+        <v>2021.0</v>
       </c>
       <c r="G506" s="1" t="s">
         <v>8</v>
@@ -10713,8 +10716,8 @@
       <c r="B507" s="5">
         <v>2.1765423E7</v>
       </c>
-      <c r="C507" s="9" t="s">
-        <v>15</v>
+      <c r="C507" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="D507" s="5">
         <v>1.0</v>
@@ -10722,8 +10725,8 @@
       <c r="E507" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F507" s="7">
-        <v>2021.0</v>
+      <c r="F507" s="13">
+        <v>2022.0</v>
       </c>
       <c r="G507" s="1" t="s">
         <v>16</v>
@@ -10734,7 +10737,7 @@
         <v>2.1765423E7</v>
       </c>
       <c r="C508" s="4" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="D508" s="5">
         <v>1.0</v>
@@ -10743,7 +10746,7 @@
         <v>7</v>
       </c>
       <c r="F508" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G508" s="2" t="s">
         <v>19</v>
@@ -10754,7 +10757,7 @@
         <v>2.1765423E7</v>
       </c>
       <c r="C509" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D509" s="5">
         <v>1.0</v>
@@ -10763,7 +10766,7 @@
         <v>7</v>
       </c>
       <c r="F509" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G509" s="2" t="s">
         <v>19</v>
@@ -10774,7 +10777,7 @@
         <v>2.1765423E7</v>
       </c>
       <c r="C510" s="4" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="D510" s="5">
         <v>1.0</v>
@@ -10783,7 +10786,7 @@
         <v>14</v>
       </c>
       <c r="F510" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G510" s="2" t="s">
         <v>27</v>
@@ -10794,10 +10797,10 @@
         <v>2.0387129E7</v>
       </c>
       <c r="C511" s="4" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="D511" s="5">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="E511" s="4" t="s">
         <v>14</v>
@@ -10813,17 +10816,17 @@
       <c r="B512" s="5">
         <v>2.0387129E7</v>
       </c>
-      <c r="C512" s="6" t="s">
-        <v>56</v>
+      <c r="C512" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="D512" s="5">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E512" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F512" s="5">
-        <v>2023.0</v>
+        <v>2021.0</v>
       </c>
       <c r="G512" s="1" t="s">
         <v>8</v>
@@ -10834,7 +10837,7 @@
         <v>2.0387129E7</v>
       </c>
       <c r="C513" s="4" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="D513" s="5">
         <v>1.0</v>
@@ -10843,7 +10846,7 @@
         <v>14</v>
       </c>
       <c r="F513" s="5">
-        <v>2020.0</v>
+        <v>2021.0</v>
       </c>
       <c r="G513" s="1" t="s">
         <v>8</v>
@@ -10853,8 +10856,8 @@
       <c r="B514" s="5">
         <v>2.0387129E7</v>
       </c>
-      <c r="C514" s="9" t="s">
-        <v>15</v>
+      <c r="C514" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="D514" s="5">
         <v>1.0</v>
@@ -10862,8 +10865,8 @@
       <c r="E514" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F514" s="7">
-        <v>2021.0</v>
+      <c r="F514" s="13">
+        <v>2022.0</v>
       </c>
       <c r="G514" s="1" t="s">
         <v>16</v>
@@ -10874,7 +10877,7 @@
         <v>2.0387129E7</v>
       </c>
       <c r="C515" s="4" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="D515" s="5">
         <v>1.0</v>
@@ -10883,7 +10886,7 @@
         <v>7</v>
       </c>
       <c r="F515" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G515" s="2" t="s">
         <v>19</v>
@@ -10894,7 +10897,7 @@
         <v>2.0387129E7</v>
       </c>
       <c r="C516" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D516" s="5">
         <v>1.0</v>
@@ -10903,7 +10906,7 @@
         <v>7</v>
       </c>
       <c r="F516" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G516" s="2" t="s">
         <v>19</v>
@@ -10914,7 +10917,7 @@
         <v>2.0387129E7</v>
       </c>
       <c r="C517" s="4" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="D517" s="5">
         <v>1.0</v>
@@ -10923,7 +10926,7 @@
         <v>14</v>
       </c>
       <c r="F517" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G517" s="2" t="s">
         <v>27</v>
@@ -10934,10 +10937,10 @@
         <v>2.1123456E7</v>
       </c>
       <c r="C518" s="4" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="D518" s="5">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E518" s="4" t="s">
         <v>14</v>
@@ -10953,17 +10956,17 @@
       <c r="B519" s="5">
         <v>2.1123456E7</v>
       </c>
-      <c r="C519" s="6" t="s">
-        <v>56</v>
+      <c r="C519" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="D519" s="5">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E519" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F519" s="5">
-        <v>2023.0</v>
+        <v>2021.0</v>
       </c>
       <c r="G519" s="1" t="s">
         <v>8</v>
@@ -10974,7 +10977,7 @@
         <v>2.1123456E7</v>
       </c>
       <c r="C520" s="4" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="D520" s="5">
         <v>1.0</v>
@@ -10983,7 +10986,7 @@
         <v>14</v>
       </c>
       <c r="F520" s="5">
-        <v>2020.0</v>
+        <v>2021.0</v>
       </c>
       <c r="G520" s="1" t="s">
         <v>8</v>
@@ -10993,8 +10996,8 @@
       <c r="B521" s="5">
         <v>2.1123456E7</v>
       </c>
-      <c r="C521" s="9" t="s">
-        <v>15</v>
+      <c r="C521" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="D521" s="5">
         <v>1.0</v>
@@ -11002,8 +11005,8 @@
       <c r="E521" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F521" s="7">
-        <v>2021.0</v>
+      <c r="F521" s="13">
+        <v>2022.0</v>
       </c>
       <c r="G521" s="1" t="s">
         <v>16</v>
@@ -11014,7 +11017,7 @@
         <v>2.1123456E7</v>
       </c>
       <c r="C522" s="4" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="D522" s="5">
         <v>1.0</v>
@@ -11023,7 +11026,7 @@
         <v>7</v>
       </c>
       <c r="F522" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G522" s="2" t="s">
         <v>19</v>
@@ -11034,7 +11037,7 @@
         <v>2.1123456E7</v>
       </c>
       <c r="C523" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D523" s="5">
         <v>1.0</v>
@@ -11043,7 +11046,7 @@
         <v>7</v>
       </c>
       <c r="F523" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G523" s="2" t="s">
         <v>19</v>
@@ -11054,7 +11057,7 @@
         <v>2.1123456E7</v>
       </c>
       <c r="C524" s="4" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="D524" s="5">
         <v>1.0</v>
@@ -11063,7 +11066,7 @@
         <v>14</v>
       </c>
       <c r="F524" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G524" s="2" t="s">
         <v>27</v>
@@ -11074,7 +11077,7 @@
         <v>2.156789E7</v>
       </c>
       <c r="C525" s="4" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="D525" s="5">
         <v>2.0</v>
@@ -11093,17 +11096,17 @@
       <c r="B526" s="5">
         <v>2.156789E7</v>
       </c>
-      <c r="C526" s="6" t="s">
-        <v>56</v>
+      <c r="C526" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="D526" s="5">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E526" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F526" s="5">
-        <v>2023.0</v>
+        <v>2021.0</v>
       </c>
       <c r="G526" s="1" t="s">
         <v>8</v>
@@ -11114,7 +11117,7 @@
         <v>2.156789E7</v>
       </c>
       <c r="C527" s="4" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="D527" s="5">
         <v>1.0</v>
@@ -11123,7 +11126,7 @@
         <v>14</v>
       </c>
       <c r="F527" s="5">
-        <v>2020.0</v>
+        <v>2021.0</v>
       </c>
       <c r="G527" s="1" t="s">
         <v>8</v>
@@ -11133,8 +11136,8 @@
       <c r="B528" s="5">
         <v>2.156789E7</v>
       </c>
-      <c r="C528" s="9" t="s">
-        <v>15</v>
+      <c r="C528" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="D528" s="5">
         <v>1.0</v>
@@ -11142,8 +11145,8 @@
       <c r="E528" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F528" s="7">
-        <v>2021.0</v>
+      <c r="F528" s="13">
+        <v>2022.0</v>
       </c>
       <c r="G528" s="1" t="s">
         <v>16</v>
@@ -11154,7 +11157,7 @@
         <v>2.156789E7</v>
       </c>
       <c r="C529" s="4" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="D529" s="5">
         <v>1.0</v>
@@ -11163,7 +11166,7 @@
         <v>7</v>
       </c>
       <c r="F529" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G529" s="2" t="s">
         <v>19</v>
@@ -11174,7 +11177,7 @@
         <v>2.156789E7</v>
       </c>
       <c r="C530" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D530" s="5">
         <v>1.0</v>
@@ -11183,7 +11186,7 @@
         <v>7</v>
       </c>
       <c r="F530" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G530" s="2" t="s">
         <v>19</v>
@@ -11194,7 +11197,7 @@
         <v>2.156789E7</v>
       </c>
       <c r="C531" s="4" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="D531" s="5">
         <v>1.0</v>
@@ -11203,7 +11206,7 @@
         <v>14</v>
       </c>
       <c r="F531" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G531" s="2" t="s">
         <v>27</v>
@@ -11214,10 +11217,10 @@
         <v>2.1987654E7</v>
       </c>
       <c r="C532" s="4" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="D532" s="5">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="E532" s="4" t="s">
         <v>14</v>
@@ -11233,17 +11236,17 @@
       <c r="B533" s="5">
         <v>2.1987654E7</v>
       </c>
-      <c r="C533" s="6" t="s">
-        <v>56</v>
+      <c r="C533" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="D533" s="5">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E533" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F533" s="5">
-        <v>2023.0</v>
+        <v>2021.0</v>
       </c>
       <c r="G533" s="1" t="s">
         <v>8</v>
@@ -11254,7 +11257,7 @@
         <v>2.1987654E7</v>
       </c>
       <c r="C534" s="4" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="D534" s="5">
         <v>1.0</v>
@@ -11263,7 +11266,7 @@
         <v>14</v>
       </c>
       <c r="F534" s="5">
-        <v>2020.0</v>
+        <v>2021.0</v>
       </c>
       <c r="G534" s="1" t="s">
         <v>8</v>
@@ -11273,8 +11276,8 @@
       <c r="B535" s="5">
         <v>2.1987654E7</v>
       </c>
-      <c r="C535" s="9" t="s">
-        <v>15</v>
+      <c r="C535" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="D535" s="5">
         <v>1.0</v>
@@ -11282,8 +11285,8 @@
       <c r="E535" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F535" s="7">
-        <v>2021.0</v>
+      <c r="F535" s="13">
+        <v>2022.0</v>
       </c>
       <c r="G535" s="1" t="s">
         <v>16</v>
@@ -11294,7 +11297,7 @@
         <v>2.1987654E7</v>
       </c>
       <c r="C536" s="4" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="D536" s="5">
         <v>1.0</v>
@@ -11303,7 +11306,7 @@
         <v>7</v>
       </c>
       <c r="F536" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G536" s="2" t="s">
         <v>19</v>
@@ -11314,7 +11317,7 @@
         <v>2.1987654E7</v>
       </c>
       <c r="C537" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D537" s="5">
         <v>1.0</v>
@@ -11323,7 +11326,7 @@
         <v>7</v>
       </c>
       <c r="F537" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G537" s="2" t="s">
         <v>19</v>
@@ -11334,7 +11337,7 @@
         <v>2.1987654E7</v>
       </c>
       <c r="C538" s="4" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="D538" s="5">
         <v>1.0</v>
@@ -11343,7 +11346,7 @@
         <v>14</v>
       </c>
       <c r="F538" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G538" s="2" t="s">
         <v>27</v>
@@ -11354,10 +11357,10 @@
         <v>2.0654321E7</v>
       </c>
       <c r="C539" s="4" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="D539" s="5">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="E539" s="4" t="s">
         <v>14</v>
@@ -11373,17 +11376,17 @@
       <c r="B540" s="5">
         <v>2.0654321E7</v>
       </c>
-      <c r="C540" s="6" t="s">
-        <v>56</v>
+      <c r="C540" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="D540" s="5">
         <v>1.0</v>
       </c>
       <c r="E540" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F540" s="5">
-        <v>2023.0</v>
+        <v>2021.0</v>
       </c>
       <c r="G540" s="1" t="s">
         <v>8</v>
@@ -11394,7 +11397,7 @@
         <v>2.0654321E7</v>
       </c>
       <c r="C541" s="4" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="D541" s="5">
         <v>1.0</v>
@@ -11403,7 +11406,7 @@
         <v>14</v>
       </c>
       <c r="F541" s="5">
-        <v>2020.0</v>
+        <v>2021.0</v>
       </c>
       <c r="G541" s="1" t="s">
         <v>8</v>
@@ -11413,8 +11416,8 @@
       <c r="B542" s="5">
         <v>2.0654321E7</v>
       </c>
-      <c r="C542" s="9" t="s">
-        <v>15</v>
+      <c r="C542" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="D542" s="5">
         <v>1.0</v>
@@ -11422,8 +11425,8 @@
       <c r="E542" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F542" s="7">
-        <v>2021.0</v>
+      <c r="F542" s="13">
+        <v>2022.0</v>
       </c>
       <c r="G542" s="1" t="s">
         <v>16</v>
@@ -11434,7 +11437,7 @@
         <v>2.0654321E7</v>
       </c>
       <c r="C543" s="4" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="D543" s="5">
         <v>1.0</v>
@@ -11443,7 +11446,7 @@
         <v>7</v>
       </c>
       <c r="F543" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G543" s="2" t="s">
         <v>19</v>
@@ -11454,7 +11457,7 @@
         <v>2.0654321E7</v>
       </c>
       <c r="C544" s="4" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="D544" s="5">
         <v>1.0</v>
@@ -11463,7 +11466,7 @@
         <v>7</v>
       </c>
       <c r="F544" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G544" s="2" t="s">
         <v>19</v>
@@ -11474,7 +11477,7 @@
         <v>2.0654321E7</v>
       </c>
       <c r="C545" s="4" t="s">
-        <v>25</v>
+        <v>73</v>
       </c>
       <c r="D545" s="5">
         <v>1.0</v>
@@ -11483,7 +11486,7 @@
         <v>14</v>
       </c>
       <c r="F545" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G545" s="2" t="s">
         <v>27</v>
@@ -11494,10 +11497,10 @@
         <v>2.1345678E7</v>
       </c>
       <c r="C546" s="4" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="D546" s="5">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="E546" s="4" t="s">
         <v>14</v>
@@ -11513,17 +11516,17 @@
       <c r="B547" s="5">
         <v>2.1345678E7</v>
       </c>
-      <c r="C547" s="6" t="s">
-        <v>56</v>
+      <c r="C547" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="D547" s="5">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E547" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F547" s="5">
-        <v>2023.0</v>
+        <v>2021.0</v>
       </c>
       <c r="G547" s="1" t="s">
         <v>8</v>
@@ -11534,7 +11537,7 @@
         <v>2.1345678E7</v>
       </c>
       <c r="C548" s="4" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="D548" s="5">
         <v>1.0</v>
@@ -11543,7 +11546,7 @@
         <v>14</v>
       </c>
       <c r="F548" s="5">
-        <v>2020.0</v>
+        <v>2021.0</v>
       </c>
       <c r="G548" s="1" t="s">
         <v>8</v>
@@ -11553,8 +11556,8 @@
       <c r="B549" s="5">
         <v>2.1345678E7</v>
       </c>
-      <c r="C549" s="9" t="s">
-        <v>15</v>
+      <c r="C549" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="D549" s="5">
         <v>1.0</v>
@@ -11562,8 +11565,8 @@
       <c r="E549" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F549" s="7">
-        <v>2021.0</v>
+      <c r="F549" s="13">
+        <v>2022.0</v>
       </c>
       <c r="G549" s="1" t="s">
         <v>16</v>
@@ -11574,7 +11577,7 @@
         <v>2.1345678E7</v>
       </c>
       <c r="C550" s="4" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="D550" s="5">
         <v>1.0</v>
@@ -11583,7 +11586,7 @@
         <v>7</v>
       </c>
       <c r="F550" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G550" s="2" t="s">
         <v>19</v>
@@ -11594,7 +11597,7 @@
         <v>2.1345678E7</v>
       </c>
       <c r="C551" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D551" s="5">
         <v>1.0</v>
@@ -11603,7 +11606,7 @@
         <v>7</v>
       </c>
       <c r="F551" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G551" s="2" t="s">
         <v>19</v>
@@ -11614,7 +11617,7 @@
         <v>2.1345678E7</v>
       </c>
       <c r="C552" s="4" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="D552" s="5">
         <v>1.0</v>
@@ -11623,7 +11626,7 @@
         <v>14</v>
       </c>
       <c r="F552" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G552" s="2" t="s">
         <v>27</v>
@@ -11633,17 +11636,17 @@
       <c r="B553" s="5">
         <v>2.1345678E7</v>
       </c>
-      <c r="C553" s="6" t="s">
-        <v>86</v>
+      <c r="C553" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="D553" s="5">
         <v>1.0</v>
       </c>
       <c r="E553" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F553" s="5">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="G553" s="12" t="s">
         <v>32</v>
@@ -11654,16 +11657,16 @@
         <v>2.1345678E7</v>
       </c>
       <c r="C554" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D554" s="5">
         <v>1.0</v>
       </c>
       <c r="E554" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F554" s="5">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="G554" s="12" t="s">
         <v>32</v>
@@ -11674,7 +11677,7 @@
         <v>1.1111222E7</v>
       </c>
       <c r="C555" s="4" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="D555" s="5">
         <v>3.0</v>
@@ -11693,17 +11696,17 @@
       <c r="B556" s="5">
         <v>1.1111222E7</v>
       </c>
-      <c r="C556" s="6" t="s">
-        <v>56</v>
+      <c r="C556" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="D556" s="5">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E556" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F556" s="5">
-        <v>2023.0</v>
+        <v>2021.0</v>
       </c>
       <c r="G556" s="1" t="s">
         <v>8</v>
@@ -11714,16 +11717,16 @@
         <v>1.1111222E7</v>
       </c>
       <c r="C557" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D557" s="5">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="E557" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F557" s="5">
-        <v>2020.0</v>
+        <v>2021.0</v>
       </c>
       <c r="G557" s="1" t="s">
         <v>8</v>
@@ -11733,8 +11736,8 @@
       <c r="B558" s="5">
         <v>1.1111222E7</v>
       </c>
-      <c r="C558" s="9" t="s">
-        <v>15</v>
+      <c r="C558" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="D558" s="5">
         <v>1.0</v>
@@ -11742,8 +11745,8 @@
       <c r="E558" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F558" s="7">
-        <v>2021.0</v>
+      <c r="F558" s="13">
+        <v>2022.0</v>
       </c>
       <c r="G558" s="1" t="s">
         <v>16</v>
@@ -11754,7 +11757,7 @@
         <v>1.1111222E7</v>
       </c>
       <c r="C559" s="4" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="D559" s="5">
         <v>1.0</v>
@@ -11763,7 +11766,7 @@
         <v>7</v>
       </c>
       <c r="F559" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G559" s="2" t="s">
         <v>19</v>
@@ -11774,7 +11777,7 @@
         <v>1.1111222E7</v>
       </c>
       <c r="C560" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D560" s="5">
         <v>1.0</v>
@@ -11783,7 +11786,7 @@
         <v>7</v>
       </c>
       <c r="F560" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G560" s="2" t="s">
         <v>19</v>
@@ -11794,7 +11797,7 @@
         <v>1.1111222E7</v>
       </c>
       <c r="C561" s="4" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="D561" s="5">
         <v>1.0</v>
@@ -11803,7 +11806,7 @@
         <v>14</v>
       </c>
       <c r="F561" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G561" s="2" t="s">
         <v>27</v>
@@ -11813,17 +11816,17 @@
       <c r="B562" s="5">
         <v>1.1111222E7</v>
       </c>
-      <c r="C562" s="6" t="s">
-        <v>86</v>
+      <c r="C562" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="D562" s="5">
         <v>1.0</v>
       </c>
       <c r="E562" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F562" s="5">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="G562" s="12" t="s">
         <v>32</v>
@@ -11833,17 +11836,17 @@
       <c r="B563" s="5">
         <v>1.1111222E7</v>
       </c>
-      <c r="C563" s="6" t="s">
-        <v>45</v>
+      <c r="C563" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="D563" s="5">
         <v>1.0</v>
       </c>
       <c r="E563" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F563" s="5">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="G563" s="12" t="s">
         <v>32</v>
@@ -11854,10 +11857,10 @@
         <v>2.2223333E7</v>
       </c>
       <c r="C564" s="4" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="D564" s="5">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="E564" s="4" t="s">
         <v>14</v>
@@ -11873,17 +11876,17 @@
       <c r="B565" s="1">
         <v>2.2223333E7</v>
       </c>
-      <c r="C565" s="6" t="s">
-        <v>56</v>
+      <c r="C565" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="D565" s="5">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E565" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F565" s="5">
-        <v>2023.0</v>
+        <v>2021.0</v>
       </c>
       <c r="G565" s="1" t="s">
         <v>8</v>
@@ -11894,7 +11897,7 @@
         <v>2.2223333E7</v>
       </c>
       <c r="C566" s="4" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="D566" s="5">
         <v>1.0</v>
@@ -11903,7 +11906,7 @@
         <v>14</v>
       </c>
       <c r="F566" s="5">
-        <v>2020.0</v>
+        <v>2021.0</v>
       </c>
       <c r="G566" s="1" t="s">
         <v>8</v>
@@ -11913,8 +11916,8 @@
       <c r="B567" s="1">
         <v>2.2223333E7</v>
       </c>
-      <c r="C567" s="9" t="s">
-        <v>15</v>
+      <c r="C567" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="D567" s="5">
         <v>1.0</v>
@@ -11922,8 +11925,8 @@
       <c r="E567" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F567" s="7">
-        <v>2021.0</v>
+      <c r="F567" s="13">
+        <v>2022.0</v>
       </c>
       <c r="G567" s="1" t="s">
         <v>16</v>
@@ -11934,7 +11937,7 @@
         <v>2.2223333E7</v>
       </c>
       <c r="C568" s="4" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="D568" s="5">
         <v>1.0</v>
@@ -11943,7 +11946,7 @@
         <v>7</v>
       </c>
       <c r="F568" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G568" s="2" t="s">
         <v>19</v>
@@ -11954,7 +11957,7 @@
         <v>2.2223333E7</v>
       </c>
       <c r="C569" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D569" s="5">
         <v>1.0</v>
@@ -11963,7 +11966,7 @@
         <v>7</v>
       </c>
       <c r="F569" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G569" s="2" t="s">
         <v>19</v>
@@ -11974,7 +11977,7 @@
         <v>2.2223333E7</v>
       </c>
       <c r="C570" s="4" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="D570" s="5">
         <v>1.0</v>
@@ -11983,7 +11986,7 @@
         <v>14</v>
       </c>
       <c r="F570" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G570" s="2" t="s">
         <v>27</v>
@@ -11993,17 +11996,17 @@
       <c r="B571" s="1">
         <v>2.2223333E7</v>
       </c>
-      <c r="C571" s="6" t="s">
-        <v>86</v>
+      <c r="C571" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="D571" s="5">
         <v>1.0</v>
       </c>
       <c r="E571" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F571" s="5">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="G571" s="12" t="s">
         <v>32</v>
@@ -12014,16 +12017,16 @@
         <v>2.2223333E7</v>
       </c>
       <c r="C572" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D572" s="5">
         <v>1.0</v>
       </c>
       <c r="E572" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F572" s="5">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="G572" s="12" t="s">
         <v>32</v>
@@ -12034,10 +12037,10 @@
         <v>3.3334444E7</v>
       </c>
       <c r="C573" s="4" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="D573" s="5">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="E573" s="4" t="s">
         <v>14</v>
@@ -12053,17 +12056,17 @@
       <c r="B574" s="5">
         <v>3.3334444E7</v>
       </c>
-      <c r="C574" s="6" t="s">
-        <v>56</v>
+      <c r="C574" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="D574" s="5">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E574" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F574" s="5">
-        <v>2023.0</v>
+        <v>2021.0</v>
       </c>
       <c r="G574" s="1" t="s">
         <v>8</v>
@@ -12074,7 +12077,7 @@
         <v>3.3334444E7</v>
       </c>
       <c r="C575" s="4" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="D575" s="5">
         <v>1.0</v>
@@ -12083,7 +12086,7 @@
         <v>14</v>
       </c>
       <c r="F575" s="5">
-        <v>2020.0</v>
+        <v>2021.0</v>
       </c>
       <c r="G575" s="1" t="s">
         <v>8</v>
@@ -12093,8 +12096,8 @@
       <c r="B576" s="5">
         <v>3.3334444E7</v>
       </c>
-      <c r="C576" s="9" t="s">
-        <v>15</v>
+      <c r="C576" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="D576" s="5">
         <v>1.0</v>
@@ -12102,8 +12105,8 @@
       <c r="E576" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F576" s="7">
-        <v>2021.0</v>
+      <c r="F576" s="13">
+        <v>2022.0</v>
       </c>
       <c r="G576" s="1" t="s">
         <v>16</v>
@@ -12114,7 +12117,7 @@
         <v>3.3334444E7</v>
       </c>
       <c r="C577" s="4" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="D577" s="5">
         <v>1.0</v>
@@ -12123,7 +12126,7 @@
         <v>7</v>
       </c>
       <c r="F577" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G577" s="2" t="s">
         <v>19</v>
@@ -12134,7 +12137,7 @@
         <v>3.3334444E7</v>
       </c>
       <c r="C578" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D578" s="5">
         <v>1.0</v>
@@ -12143,7 +12146,7 @@
         <v>7</v>
       </c>
       <c r="F578" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G578" s="2" t="s">
         <v>19</v>
@@ -12154,7 +12157,7 @@
         <v>3.3334444E7</v>
       </c>
       <c r="C579" s="4" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="D579" s="5">
         <v>1.0</v>
@@ -12163,7 +12166,7 @@
         <v>14</v>
       </c>
       <c r="F579" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G579" s="2" t="s">
         <v>27</v>
@@ -12173,17 +12176,17 @@
       <c r="B580" s="5">
         <v>3.3334444E7</v>
       </c>
-      <c r="C580" s="6" t="s">
-        <v>86</v>
+      <c r="C580" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="D580" s="5">
         <v>1.0</v>
       </c>
       <c r="E580" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F580" s="5">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="G580" s="12" t="s">
         <v>32</v>
@@ -12194,16 +12197,16 @@
         <v>3.3334444E7</v>
       </c>
       <c r="C581" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D581" s="5">
         <v>1.0</v>
       </c>
       <c r="E581" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F581" s="5">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="G581" s="12" t="s">
         <v>32</v>
@@ -13451,13 +13454,13 @@
     </row>
     <row r="644" ht="15.75" customHeight="1">
       <c r="B644" s="5">
-        <v>2.2223333E7</v>
+        <v>2.1479513E7</v>
       </c>
       <c r="C644" s="4" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="D644" s="5">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="E644" s="4" t="s">
         <v>14</v>
@@ -13465,8 +13468,8 @@
       <c r="F644" s="5">
         <v>2022.0</v>
       </c>
-      <c r="G644" s="1" t="s">
-        <v>16</v>
+      <c r="G644" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="645" ht="15.75" customHeight="1">
@@ -13474,10 +13477,10 @@
         <v>2.1479513E7</v>
       </c>
       <c r="C645" s="4" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D645" s="5">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E645" s="4" t="s">
         <v>14</v>
@@ -13494,10 +13497,10 @@
         <v>2.1479513E7</v>
       </c>
       <c r="C646" s="4" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="D646" s="5">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="E646" s="4" t="s">
         <v>14</v>
@@ -13513,8 +13516,8 @@
       <c r="B647" s="5">
         <v>2.1479513E7</v>
       </c>
-      <c r="C647" s="4" t="s">
-        <v>43</v>
+      <c r="C647" s="6" t="s">
+        <v>84</v>
       </c>
       <c r="D647" s="5">
         <v>1.0</v>
@@ -13523,10 +13526,10 @@
         <v>14</v>
       </c>
       <c r="F647" s="5">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="G647" s="2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="648" ht="15.75" customHeight="1">
@@ -13534,7 +13537,7 @@
         <v>2.1479513E7</v>
       </c>
       <c r="C648" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D648" s="5">
         <v>1.0</v>
@@ -13554,7 +13557,7 @@
         <v>2.1479513E7</v>
       </c>
       <c r="C649" s="6" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="D649" s="5">
         <v>1.0</v>
@@ -13571,10 +13574,10 @@
     </row>
     <row r="650" ht="15.75" customHeight="1">
       <c r="B650" s="5">
-        <v>2.1479513E7</v>
-      </c>
-      <c r="C650" s="6" t="s">
-        <v>91</v>
+        <v>1.570238E7</v>
+      </c>
+      <c r="C650" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="D650" s="5">
         <v>1.0</v>
@@ -13583,10 +13586,10 @@
         <v>14</v>
       </c>
       <c r="F650" s="5">
-        <v>2023.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G650" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="651" ht="15.75" customHeight="1">
@@ -13594,10 +13597,10 @@
         <v>1.570238E7</v>
       </c>
       <c r="C651" s="4" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D651" s="5">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E651" s="4" t="s">
         <v>14</v>
@@ -13614,10 +13617,10 @@
         <v>1.570238E7</v>
       </c>
       <c r="C652" s="4" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="D652" s="5">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="E652" s="4" t="s">
         <v>14</v>
@@ -13633,8 +13636,8 @@
       <c r="B653" s="5">
         <v>1.570238E7</v>
       </c>
-      <c r="C653" s="4" t="s">
-        <v>43</v>
+      <c r="C653" s="6" t="s">
+        <v>84</v>
       </c>
       <c r="D653" s="5">
         <v>1.0</v>
@@ -13643,10 +13646,10 @@
         <v>14</v>
       </c>
       <c r="F653" s="5">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="G653" s="2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="654" ht="15.75" customHeight="1">
@@ -13654,7 +13657,7 @@
         <v>1.570238E7</v>
       </c>
       <c r="C654" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D654" s="5">
         <v>1.0</v>
@@ -13674,7 +13677,7 @@
         <v>1.570238E7</v>
       </c>
       <c r="C655" s="6" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="D655" s="5">
         <v>1.0</v>
@@ -13691,10 +13694,10 @@
     </row>
     <row r="656" ht="15.75" customHeight="1">
       <c r="B656" s="5">
-        <v>1.570238E7</v>
-      </c>
-      <c r="C656" s="6" t="s">
-        <v>91</v>
+        <v>1.9073284E7</v>
+      </c>
+      <c r="C656" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="D656" s="5">
         <v>1.0</v>
@@ -13703,10 +13706,10 @@
         <v>14</v>
       </c>
       <c r="F656" s="5">
-        <v>2023.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G656" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="657" ht="15.75" customHeight="1">
@@ -13714,10 +13717,10 @@
         <v>1.9073284E7</v>
       </c>
       <c r="C657" s="4" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D657" s="5">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E657" s="4" t="s">
         <v>14</v>
@@ -13734,10 +13737,10 @@
         <v>1.9073284E7</v>
       </c>
       <c r="C658" s="4" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="D658" s="5">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="E658" s="4" t="s">
         <v>14</v>
@@ -13753,8 +13756,8 @@
       <c r="B659" s="5">
         <v>1.9073284E7</v>
       </c>
-      <c r="C659" s="4" t="s">
-        <v>43</v>
+      <c r="C659" s="6" t="s">
+        <v>84</v>
       </c>
       <c r="D659" s="5">
         <v>1.0</v>
@@ -13763,10 +13766,10 @@
         <v>14</v>
       </c>
       <c r="F659" s="5">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="G659" s="2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="660" ht="15.75" customHeight="1">
@@ -13774,7 +13777,7 @@
         <v>1.9073284E7</v>
       </c>
       <c r="C660" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D660" s="5">
         <v>1.0</v>
@@ -13794,7 +13797,7 @@
         <v>1.9073284E7</v>
       </c>
       <c r="C661" s="6" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="D661" s="5">
         <v>1.0</v>
@@ -13811,10 +13814,10 @@
     </row>
     <row r="662" ht="15.75" customHeight="1">
       <c r="B662" s="5">
-        <v>1.9073284E7</v>
-      </c>
-      <c r="C662" s="6" t="s">
-        <v>91</v>
+        <v>1.6134702E7</v>
+      </c>
+      <c r="C662" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="D662" s="5">
         <v>1.0</v>
@@ -13823,10 +13826,10 @@
         <v>14</v>
       </c>
       <c r="F662" s="5">
-        <v>2023.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G662" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="663" ht="15.75" customHeight="1">
@@ -13834,10 +13837,10 @@
         <v>1.6134702E7</v>
       </c>
       <c r="C663" s="4" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D663" s="5">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E663" s="4" t="s">
         <v>14</v>
@@ -13854,10 +13857,10 @@
         <v>1.6134702E7</v>
       </c>
       <c r="C664" s="4" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="D664" s="5">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="E664" s="4" t="s">
         <v>14</v>
@@ -13873,8 +13876,8 @@
       <c r="B665" s="5">
         <v>1.6134702E7</v>
       </c>
-      <c r="C665" s="4" t="s">
-        <v>43</v>
+      <c r="C665" s="6" t="s">
+        <v>84</v>
       </c>
       <c r="D665" s="5">
         <v>1.0</v>
@@ -13883,10 +13886,10 @@
         <v>14</v>
       </c>
       <c r="F665" s="5">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="G665" s="2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="666" ht="15.75" customHeight="1">
@@ -13894,7 +13897,7 @@
         <v>1.6134702E7</v>
       </c>
       <c r="C666" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D666" s="5">
         <v>1.0</v>
@@ -13914,7 +13917,7 @@
         <v>1.6134702E7</v>
       </c>
       <c r="C667" s="6" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="D667" s="5">
         <v>1.0</v>
@@ -13931,33 +13934,33 @@
     </row>
     <row r="668" ht="15.75" customHeight="1">
       <c r="B668" s="5">
-        <v>1.6134702E7</v>
-      </c>
-      <c r="C668" s="6" t="s">
-        <v>91</v>
+        <v>1.1112222E7</v>
+      </c>
+      <c r="C668" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="D668" s="5">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="E668" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F668" s="5">
-        <v>2023.0</v>
-      </c>
-      <c r="G668" s="2" t="s">
-        <v>16</v>
+        <v>2022.0</v>
+      </c>
+      <c r="G668" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="669" ht="15.75" customHeight="1">
-      <c r="B669" s="5">
-        <v>1.1112222E7</v>
-      </c>
-      <c r="C669" s="4" t="s">
-        <v>22</v>
+      <c r="B669" s="2">
+        <v>2.2213333E7</v>
+      </c>
+      <c r="C669" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="D669" s="5">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="E669" s="4" t="s">
         <v>13</v>
@@ -13966,18 +13969,18 @@
         <v>2022.0</v>
       </c>
       <c r="G669" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="670" ht="15.75" customHeight="1">
-      <c r="B670" s="5">
-        <v>2.2223333E7</v>
-      </c>
-      <c r="C670" s="4" t="s">
-        <v>22</v>
+      <c r="B670" s="2">
+        <v>2.2213333E7</v>
+      </c>
+      <c r="C670" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="D670" s="5">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="E670" s="4" t="s">
         <v>13</v>
@@ -13986,7 +13989,7 @@
         <v>2022.0</v>
       </c>
       <c r="G670" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="671" ht="15.75" customHeight="1">
@@ -13994,7 +13997,7 @@
         <v>2.2213333E7</v>
       </c>
       <c r="C671" s="6" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D671" s="5">
         <v>1.0</v>
@@ -14014,7 +14017,7 @@
         <v>2.2213333E7</v>
       </c>
       <c r="C672" s="6" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="D672" s="5">
         <v>1.0</v>
@@ -14025,7 +14028,7 @@
       <c r="F672" s="5">
         <v>2022.0</v>
       </c>
-      <c r="G672" s="1" t="s">
+      <c r="G672" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -14033,88 +14036,88 @@
       <c r="B673" s="2">
         <v>2.2213333E7</v>
       </c>
-      <c r="C673" s="6" t="s">
-        <v>49</v>
+      <c r="C673" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="D673" s="5">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E673" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F673" s="5">
         <v>2022.0</v>
       </c>
-      <c r="G673" s="1" t="s">
-        <v>8</v>
+      <c r="G673" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="674" ht="15.75" customHeight="1">
       <c r="B674" s="2">
         <v>2.2213333E7</v>
       </c>
-      <c r="C674" s="6" t="s">
-        <v>87</v>
+      <c r="C674" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="D674" s="5">
         <v>1.0</v>
       </c>
       <c r="E674" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F674" s="5">
         <v>2022.0</v>
       </c>
       <c r="G674" s="2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="675" ht="15.75" customHeight="1">
       <c r="B675" s="2">
         <v>2.2213333E7</v>
       </c>
-      <c r="C675" s="4" t="s">
-        <v>51</v>
+      <c r="C675" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="D675" s="5">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="E675" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F675" s="5">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="G675" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="676" ht="15.75" customHeight="1">
       <c r="B676" s="2">
         <v>2.2213333E7</v>
       </c>
-      <c r="C676" s="4" t="s">
-        <v>52</v>
+      <c r="C676" s="6" t="s">
+        <v>89</v>
       </c>
       <c r="D676" s="5">
         <v>1.0</v>
       </c>
       <c r="E676" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F676" s="5">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="G676" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="677" ht="15.75" customHeight="1">
       <c r="B677" s="2">
-        <v>2.2213333E7</v>
+        <v>3.3834444E7</v>
       </c>
       <c r="C677" s="6" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="D677" s="5">
         <v>1.0</v>
@@ -14123,18 +14126,18 @@
         <v>13</v>
       </c>
       <c r="F677" s="5">
-        <v>2023.0</v>
-      </c>
-      <c r="G677" s="2" t="s">
-        <v>19</v>
+        <v>2022.0</v>
+      </c>
+      <c r="G677" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="678" ht="15.75" customHeight="1">
       <c r="B678" s="2">
-        <v>2.2213333E7</v>
+        <v>3.3834444E7</v>
       </c>
       <c r="C678" s="6" t="s">
-        <v>89</v>
+        <v>29</v>
       </c>
       <c r="D678" s="5">
         <v>1.0</v>
@@ -14143,10 +14146,10 @@
         <v>13</v>
       </c>
       <c r="F678" s="5">
-        <v>2023.0</v>
-      </c>
-      <c r="G678" s="2" t="s">
-        <v>19</v>
+        <v>2022.0</v>
+      </c>
+      <c r="G678" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="679" ht="15.75" customHeight="1">
@@ -14154,7 +14157,7 @@
         <v>3.3834444E7</v>
       </c>
       <c r="C679" s="6" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D679" s="5">
         <v>1.0</v>
@@ -14174,7 +14177,7 @@
         <v>3.3834444E7</v>
       </c>
       <c r="C680" s="6" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="D680" s="5">
         <v>1.0</v>
@@ -14185,7 +14188,7 @@
       <c r="F680" s="5">
         <v>2022.0</v>
       </c>
-      <c r="G680" s="1" t="s">
+      <c r="G680" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -14193,131 +14196,131 @@
       <c r="B681" s="2">
         <v>3.3834444E7</v>
       </c>
-      <c r="C681" s="6" t="s">
-        <v>49</v>
+      <c r="C681" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="D681" s="5">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E681" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F681" s="5">
         <v>2022.0</v>
       </c>
-      <c r="G681" s="1" t="s">
-        <v>8</v>
+      <c r="G681" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="682" ht="15.75" customHeight="1">
       <c r="B682" s="2">
         <v>3.3834444E7</v>
       </c>
-      <c r="C682" s="6" t="s">
-        <v>87</v>
+      <c r="C682" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="D682" s="5">
         <v>1.0</v>
       </c>
       <c r="E682" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F682" s="5">
         <v>2022.0</v>
       </c>
       <c r="G682" s="2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="683" ht="15.75" customHeight="1">
       <c r="B683" s="2">
         <v>3.3834444E7</v>
       </c>
-      <c r="C683" s="4" t="s">
-        <v>51</v>
+      <c r="C683" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="D683" s="5">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="E683" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F683" s="5">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="G683" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="684" ht="15.75" customHeight="1">
       <c r="B684" s="2">
         <v>3.3834444E7</v>
       </c>
-      <c r="C684" s="4" t="s">
-        <v>52</v>
+      <c r="C684" s="6" t="s">
+        <v>89</v>
       </c>
       <c r="D684" s="5">
         <v>1.0</v>
       </c>
       <c r="E684" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F684" s="5">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="G684" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="685" ht="15.75" customHeight="1">
-      <c r="B685" s="2">
-        <v>3.3834444E7</v>
-      </c>
-      <c r="C685" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D685" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="E685" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F685" s="5">
-        <v>2023.0</v>
-      </c>
-      <c r="G685" s="2" t="s">
-        <v>19</v>
+      <c r="B685" s="1">
+        <v>1.7829051E7</v>
+      </c>
+      <c r="C685" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D685" s="11">
+        <v>3.0</v>
+      </c>
+      <c r="E685" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F685" s="11">
+        <v>2019.0</v>
+      </c>
+      <c r="G685" s="12" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="686" ht="15.75" customHeight="1">
-      <c r="B686" s="2">
-        <v>3.3834444E7</v>
-      </c>
-      <c r="C686" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D686" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="E686" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F686" s="5">
-        <v>2023.0</v>
-      </c>
-      <c r="G686" s="2" t="s">
-        <v>19</v>
+      <c r="B686" s="1">
+        <v>1.7829051E7</v>
+      </c>
+      <c r="C686" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D686" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="E686" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F686" s="11">
+        <v>2019.0</v>
+      </c>
+      <c r="G686" s="12" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="687" ht="15.75" customHeight="1">
       <c r="B687" s="1">
         <v>1.7829051E7</v>
       </c>
-      <c r="C687" s="10" t="s">
-        <v>15</v>
+      <c r="C687" s="14" t="s">
+        <v>56</v>
       </c>
       <c r="D687" s="11">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="E687" s="10" t="s">
         <v>14</v>
@@ -14334,39 +14337,39 @@
         <v>1.7829051E7</v>
       </c>
       <c r="C688" s="10" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="D688" s="11">
         <v>1.0</v>
       </c>
       <c r="E688" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F688" s="11">
-        <v>2019.0</v>
+        <v>2020.0</v>
       </c>
       <c r="G688" s="12" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="689" ht="15.75" customHeight="1">
       <c r="B689" s="1">
         <v>1.7829051E7</v>
       </c>
-      <c r="C689" s="13" t="s">
-        <v>56</v>
+      <c r="C689" s="10" t="s">
+        <v>22</v>
       </c>
       <c r="D689" s="11">
         <v>1.0</v>
       </c>
       <c r="E689" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F689" s="11">
-        <v>2019.0</v>
+        <v>2020.0</v>
       </c>
       <c r="G689" s="12" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="690" ht="15.75" customHeight="1">
@@ -14374,19 +14377,19 @@
         <v>1.7829051E7</v>
       </c>
       <c r="C690" s="10" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="D690" s="11">
         <v>1.0</v>
       </c>
       <c r="E690" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F690" s="11">
         <v>2020.0</v>
       </c>
       <c r="G690" s="12" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="691" ht="15.75" customHeight="1">
@@ -14394,19 +14397,19 @@
         <v>1.7829051E7</v>
       </c>
       <c r="C691" s="10" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="D691" s="11">
         <v>1.0</v>
       </c>
       <c r="E691" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F691" s="11">
         <v>2020.0</v>
       </c>
       <c r="G691" s="12" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="692" ht="15.75" customHeight="1">
@@ -14414,19 +14417,19 @@
         <v>1.7829051E7</v>
       </c>
       <c r="C692" s="10" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="D692" s="11">
         <v>1.0</v>
       </c>
       <c r="E692" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F692" s="11">
-        <v>2020.0</v>
+        <v>2021.0</v>
       </c>
       <c r="G692" s="12" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="693" ht="15.75" customHeight="1">
@@ -14434,19 +14437,19 @@
         <v>1.7829051E7</v>
       </c>
       <c r="C693" s="10" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="D693" s="11">
         <v>1.0</v>
       </c>
       <c r="E693" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F693" s="11">
-        <v>2020.0</v>
+        <v>2021.0</v>
       </c>
       <c r="G693" s="12" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="694" ht="15.75" customHeight="1">
@@ -14454,19 +14457,19 @@
         <v>1.7829051E7</v>
       </c>
       <c r="C694" s="10" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D694" s="11">
         <v>1.0</v>
       </c>
       <c r="E694" s="10" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F694" s="11">
         <v>2021.0</v>
       </c>
       <c r="G694" s="12" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="695" ht="15.75" customHeight="1">
@@ -14474,19 +14477,19 @@
         <v>1.7829051E7</v>
       </c>
       <c r="C695" s="10" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D695" s="11">
         <v>1.0</v>
       </c>
       <c r="E695" s="10" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F695" s="11">
         <v>2021.0</v>
       </c>
       <c r="G695" s="12" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="696" ht="15.75" customHeight="1">
@@ -14494,19 +14497,19 @@
         <v>1.7829051E7</v>
       </c>
       <c r="C696" s="10" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D696" s="11">
         <v>1.0</v>
       </c>
       <c r="E696" s="10" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F696" s="11">
         <v>2021.0</v>
       </c>
       <c r="G696" s="12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="697" ht="15.75" customHeight="1">
@@ -14514,19 +14517,19 @@
         <v>1.7829051E7</v>
       </c>
       <c r="C697" s="10" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="D697" s="11">
         <v>1.0</v>
       </c>
       <c r="E697" s="10" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F697" s="11">
         <v>2021.0</v>
       </c>
       <c r="G697" s="12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="698" ht="15.75" customHeight="1">
@@ -14534,19 +14537,19 @@
         <v>1.7829051E7</v>
       </c>
       <c r="C698" s="10" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="D698" s="11">
         <v>1.0</v>
       </c>
       <c r="E698" s="10" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F698" s="11">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G698" s="12" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
     </row>
     <row r="699" ht="15.75" customHeight="1">
@@ -14554,110 +14557,110 @@
         <v>1.7829051E7</v>
       </c>
       <c r="C699" s="10" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="D699" s="11">
         <v>1.0</v>
       </c>
       <c r="E699" s="10" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F699" s="11">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G699" s="12" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
     </row>
     <row r="700" ht="15.75" customHeight="1">
       <c r="B700" s="1">
         <v>1.7829051E7</v>
       </c>
-      <c r="C700" s="10" t="s">
-        <v>66</v>
+      <c r="C700" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="D700" s="11">
         <v>1.0</v>
       </c>
       <c r="E700" s="10" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F700" s="11">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="G700" s="12" t="s">
-        <v>53</v>
+        <v>92</v>
       </c>
     </row>
     <row r="701" ht="15.75" customHeight="1">
       <c r="B701" s="1">
         <v>1.7829051E7</v>
       </c>
-      <c r="C701" s="10" t="s">
-        <v>73</v>
+      <c r="C701" s="14" t="s">
+        <v>81</v>
       </c>
       <c r="D701" s="11">
         <v>1.0</v>
       </c>
       <c r="E701" s="10" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F701" s="11">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="G701" s="12" t="s">
-        <v>53</v>
+        <v>92</v>
       </c>
     </row>
     <row r="702" ht="15.75" customHeight="1">
       <c r="B702" s="1">
-        <v>1.7829051E7</v>
-      </c>
-      <c r="C702" s="13" t="s">
-        <v>42</v>
+        <v>2.0571439E7</v>
+      </c>
+      <c r="C702" s="10" t="s">
+        <v>15</v>
       </c>
       <c r="D702" s="11">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="E702" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F702" s="11">
-        <v>2023.0</v>
+        <v>2019.0</v>
       </c>
       <c r="G702" s="12" t="s">
-        <v>92</v>
+        <v>8</v>
       </c>
     </row>
     <row r="703" ht="15.75" customHeight="1">
       <c r="B703" s="1">
-        <v>1.7829051E7</v>
-      </c>
-      <c r="C703" s="13" t="s">
-        <v>81</v>
+        <v>2.0571439E7</v>
+      </c>
+      <c r="C703" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="D703" s="11">
         <v>1.0</v>
       </c>
       <c r="E703" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F703" s="11">
-        <v>2023.0</v>
+        <v>2019.0</v>
       </c>
       <c r="G703" s="12" t="s">
-        <v>92</v>
+        <v>8</v>
       </c>
     </row>
     <row r="704" ht="15.75" customHeight="1">
       <c r="B704" s="1">
         <v>2.0571439E7</v>
       </c>
-      <c r="C704" s="10" t="s">
-        <v>15</v>
+      <c r="C704" s="14" t="s">
+        <v>56</v>
       </c>
       <c r="D704" s="11">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="E704" s="10" t="s">
         <v>14</v>
@@ -14674,39 +14677,39 @@
         <v>2.0571439E7</v>
       </c>
       <c r="C705" s="10" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="D705" s="11">
         <v>1.0</v>
       </c>
       <c r="E705" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F705" s="11">
-        <v>2019.0</v>
+        <v>2020.0</v>
       </c>
       <c r="G705" s="12" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="706" ht="15.75" customHeight="1">
       <c r="B706" s="1">
         <v>2.0571439E7</v>
       </c>
-      <c r="C706" s="13" t="s">
-        <v>56</v>
+      <c r="C706" s="10" t="s">
+        <v>22</v>
       </c>
       <c r="D706" s="11">
         <v>1.0</v>
       </c>
       <c r="E706" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F706" s="11">
-        <v>2019.0</v>
+        <v>2020.0</v>
       </c>
       <c r="G706" s="12" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="707" ht="15.75" customHeight="1">
@@ -14714,19 +14717,19 @@
         <v>2.0571439E7</v>
       </c>
       <c r="C707" s="10" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="D707" s="11">
         <v>1.0</v>
       </c>
       <c r="E707" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F707" s="11">
         <v>2020.0</v>
       </c>
       <c r="G707" s="12" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="708" ht="15.75" customHeight="1">
@@ -14734,19 +14737,19 @@
         <v>2.0571439E7</v>
       </c>
       <c r="C708" s="10" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="D708" s="11">
         <v>1.0</v>
       </c>
       <c r="E708" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F708" s="11">
         <v>2020.0</v>
       </c>
       <c r="G708" s="12" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="709" ht="15.75" customHeight="1">
@@ -14754,19 +14757,19 @@
         <v>2.0571439E7</v>
       </c>
       <c r="C709" s="10" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="D709" s="11">
         <v>1.0</v>
       </c>
       <c r="E709" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F709" s="11">
-        <v>2020.0</v>
+        <v>2021.0</v>
       </c>
       <c r="G709" s="12" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="710" ht="15.75" customHeight="1">
@@ -14774,19 +14777,19 @@
         <v>2.0571439E7</v>
       </c>
       <c r="C710" s="10" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="D710" s="11">
         <v>1.0</v>
       </c>
       <c r="E710" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F710" s="11">
-        <v>2020.0</v>
+        <v>2021.0</v>
       </c>
       <c r="G710" s="12" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="711" ht="15.75" customHeight="1">
@@ -14794,19 +14797,19 @@
         <v>2.0571439E7</v>
       </c>
       <c r="C711" s="10" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D711" s="11">
         <v>1.0</v>
       </c>
       <c r="E711" s="10" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F711" s="11">
         <v>2021.0</v>
       </c>
       <c r="G711" s="12" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="712" ht="15.75" customHeight="1">
@@ -14814,19 +14817,19 @@
         <v>2.0571439E7</v>
       </c>
       <c r="C712" s="10" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D712" s="11">
         <v>1.0</v>
       </c>
       <c r="E712" s="10" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F712" s="11">
         <v>2021.0</v>
       </c>
       <c r="G712" s="12" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="713" ht="15.75" customHeight="1">
@@ -14834,19 +14837,19 @@
         <v>2.0571439E7</v>
       </c>
       <c r="C713" s="10" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D713" s="11">
         <v>1.0</v>
       </c>
       <c r="E713" s="10" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F713" s="11">
         <v>2021.0</v>
       </c>
       <c r="G713" s="12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="714" ht="15.75" customHeight="1">
@@ -14854,19 +14857,19 @@
         <v>2.0571439E7</v>
       </c>
       <c r="C714" s="10" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="D714" s="11">
         <v>1.0</v>
       </c>
       <c r="E714" s="10" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F714" s="11">
         <v>2021.0</v>
       </c>
       <c r="G714" s="12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="715" ht="15.75" customHeight="1">
@@ -14874,19 +14877,19 @@
         <v>2.0571439E7</v>
       </c>
       <c r="C715" s="10" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="D715" s="11">
         <v>1.0</v>
       </c>
       <c r="E715" s="10" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F715" s="11">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G715" s="12" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
     </row>
     <row r="716" ht="15.75" customHeight="1">
@@ -14894,101 +14897,63 @@
         <v>2.0571439E7</v>
       </c>
       <c r="C716" s="10" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="D716" s="11">
         <v>1.0</v>
       </c>
       <c r="E716" s="10" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F716" s="11">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="G716" s="12" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
     </row>
     <row r="717" ht="15.75" customHeight="1">
       <c r="B717" s="1">
         <v>2.0571439E7</v>
       </c>
-      <c r="C717" s="10" t="s">
-        <v>66</v>
+      <c r="C717" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="D717" s="11">
         <v>1.0</v>
       </c>
       <c r="E717" s="10" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F717" s="11">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="G717" s="12" t="s">
-        <v>53</v>
+        <v>92</v>
       </c>
     </row>
     <row r="718" ht="15.75" customHeight="1">
       <c r="B718" s="1">
         <v>2.0571439E7</v>
       </c>
-      <c r="C718" s="10" t="s">
-        <v>73</v>
+      <c r="C718" s="14" t="s">
+        <v>81</v>
       </c>
       <c r="D718" s="11">
         <v>1.0</v>
       </c>
       <c r="E718" s="10" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F718" s="11">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="G718" s="12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="719" ht="15.75" customHeight="1">
-      <c r="B719" s="1">
-        <v>2.0571439E7</v>
-      </c>
-      <c r="C719" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D719" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="E719" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F719" s="11">
-        <v>2023.0</v>
-      </c>
-      <c r="G719" s="12" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="720" ht="15.75" customHeight="1">
-      <c r="B720" s="1">
-        <v>2.0571439E7</v>
-      </c>
-      <c r="C720" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D720" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="E720" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F720" s="11">
-        <v>2023.0</v>
-      </c>
-      <c r="G720" s="12" t="s">
-        <v>92</v>
-      </c>
-    </row>
+    <row r="719" ht="15.75" customHeight="1"/>
+    <row r="720" ht="15.75" customHeight="1"/>
     <row r="721" ht="15.75" customHeight="1"/>
     <row r="722" ht="15.75" customHeight="1"/>
     <row r="723" ht="15.75" customHeight="1"/>
@@ -15469,8 +15434,6 @@
     <row r="1198" ht="15.75" customHeight="1"/>
     <row r="1199" ht="15.75" customHeight="1"/>
     <row r="1200" ht="15.75" customHeight="1"/>
-    <row r="1201" ht="15.75" customHeight="1"/>
-    <row r="1202" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>